<commit_message>
update doc file masih berjalan :+1:
</commit_message>
<xml_diff>
--- a/Learn_Web_Prosesing_Data_Excle/pfg_konversi_sc/Book1.xlsx
+++ b/Learn_Web_Prosesing_Data_Excle/pfg_konversi_sc/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_WorkingData\05_git\My_Learing_Code\Learn_Web_Prosesing_Data_Excle\pfg_konversi_sc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13A1589-37F6-484D-B80C-04D1351C7455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432251C1-5DB5-4733-8970-ADCC7C943936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A9D70391-4998-43FE-95C1-DAD7BCC1C164}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>PO</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>UK</t>
+  </si>
+  <si>
+    <t>2xl</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
   </si>
 </sst>
 </file>
@@ -467,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45108724-F681-4B97-9A65-476435B8C33F}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,14 +486,15 @@
     <col min="3" max="3" width="21.140625" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,10 +505,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -513,13 +520,16 @@
         <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -530,9 +540,6 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
@@ -544,11 +551,14 @@
       <c r="H2">
         <v>10</v>
       </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -559,9 +569,6 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
@@ -573,14 +580,17 @@
       <c r="H3">
         <v>10</v>
       </c>
-      <c r="I3">
-        <v>5</v>
+      <c r="I3" t="s">
+        <v>10</v>
       </c>
       <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -591,9 +601,6 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
         <v>14</v>
       </c>
       <c r="F4" t="s">
@@ -605,14 +612,17 @@
       <c r="H4">
         <v>10</v>
       </c>
-      <c r="I4">
-        <v>5</v>
+      <c r="I4" t="s">
+        <v>10</v>
       </c>
       <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -623,9 +633,6 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="F5" t="s">
@@ -637,14 +644,17 @@
       <c r="H5">
         <v>10</v>
       </c>
-      <c r="I5">
-        <v>5</v>
+      <c r="I5" t="s">
+        <v>10</v>
       </c>
       <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -655,9 +665,6 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
@@ -669,14 +676,17 @@
       <c r="H6">
         <v>10</v>
       </c>
-      <c r="I6">
-        <v>5</v>
+      <c r="I6" t="s">
+        <v>10</v>
       </c>
       <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -687,9 +697,6 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="F7" t="s">
@@ -701,14 +708,17 @@
       <c r="H7">
         <v>10</v>
       </c>
-      <c r="I7">
-        <v>5</v>
+      <c r="I7" t="s">
+        <v>10</v>
       </c>
       <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -719,9 +729,6 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
         <v>14</v>
       </c>
       <c r="F8" t="s">
@@ -733,10 +740,45 @@
       <c r="H8">
         <v>10</v>
       </c>
-      <c r="I8">
-        <v>5</v>
+      <c r="I8" t="s">
+        <v>10</v>
       </c>
       <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
         <v>0</v>
       </c>
     </row>

</xml_diff>